<commit_message>
Improvements in the coverage of the project
</commit_message>
<xml_diff>
--- a/utest/files/example.xlsx
+++ b/utest/files/example.xlsx
@@ -53,8 +53,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -121,12 +122,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,7 +261,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A101" activeCellId="0" sqref="A101"/>
+      <selection pane="topLeft" activeCell="I101" activeCellId="0" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -326,6 +331,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
+        <f aca="false">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
@@ -3191,8 +3197,8 @@
       <c r="H101" s="1" t="n">
         <v>12800</v>
       </c>
-      <c r="I101" s="1" t="n">
-        <v>25600</v>
+      <c r="I101" s="2" t="n">
+        <v>45323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>